<commit_message>
updated teching in faculty
</commit_message>
<xml_diff>
--- a/public/Data/faculty.xlsx
+++ b/public/Data/faculty.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FS Projects\CSE\public\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaushik\OneDrive\Desktop\department\CSE\public\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4F9965-D867-41E1-A00A-86B217D13CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A15574E-609E-4F76-A16C-2346C01462CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="434">
   <si>
     <t>S.NO.</t>
   </si>
@@ -1319,6 +1319,9 @@
   </si>
   <si>
     <t>4th  Oct 2021</t>
+  </si>
+  <si>
+    <t>empId</t>
   </si>
 </sst>
 </file>
@@ -1935,7 +1938,7 @@
   <dimension ref="A1:F114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1953,7 +1956,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>433</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
small changes in faculty excel sheet
</commit_message>
<xml_diff>
--- a/public/Data/faculty.xlsx
+++ b/public/Data/faculty.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaushik\OneDrive\Desktop\department\CSE\public\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A15574E-609E-4F76-A16C-2346C01462CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6738AF57-4D2E-4CCD-8742-E0514AAB261C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="431">
   <si>
     <t>S.NO.</t>
   </si>
   <si>
-    <t>EMP. ID</t>
-  </si>
-  <si>
     <t>Name of the Staff Member</t>
   </si>
   <si>
@@ -1246,9 +1243,6 @@
     <t>6th Feb 2025</t>
   </si>
   <si>
-    <t xml:space="preserve"> Computer Science &amp; Business System (CSBS)</t>
-  </si>
-  <si>
     <t>CVRCSEF261</t>
   </si>
   <si>
@@ -1280,9 +1274,6 @@
   </si>
   <si>
     <t>1st Sept 2022</t>
-  </si>
-  <si>
-    <t>M.Tech (Artificial Intelligence &amp; Machine Learning)</t>
   </si>
   <si>
     <t>CVRCSEF133</t>
@@ -1376,7 +1367,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1502,32 +1493,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color rgb="FFC6C6C6"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="thin">
         <color rgb="FF000000"/>
@@ -1541,7 +1506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1597,7 +1562,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1610,24 +1575,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1935,10 +1882,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F114"/>
+  <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1956,19 +1903,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1976,19 +1923,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1996,17 +1943,17 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2014,19 +1961,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2034,17 +1981,17 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2052,19 +1999,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2072,19 +2019,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2092,19 +2039,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="F8" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2112,19 +2059,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2132,19 +2079,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2152,19 +2099,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="7" t="s">
+      <c r="F11" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2172,19 +2119,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>54</v>
-      </c>
       <c r="F12" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2192,19 +2139,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="D13" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="F13" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2212,19 +2159,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="D14" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2232,19 +2179,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="D15" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>68</v>
-      </c>
       <c r="F15" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2252,19 +2199,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="D16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="7" t="s">
+      <c r="F16" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2272,19 +2219,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="F17" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2292,19 +2239,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="D18" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="E18" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="F18" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2312,17 +2259,17 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="D19" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2330,19 +2277,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E20" s="7" t="s">
+      <c r="F20" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2350,19 +2297,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E21" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2370,19 +2317,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D22" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22" s="7" t="s">
+      <c r="F22" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2390,19 +2337,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="D23" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E23" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2410,19 +2357,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="D24" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E24" s="7" t="s">
+      <c r="F24" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2430,19 +2377,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="D25" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E25" s="7" t="s">
+      <c r="F25" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2450,19 +2397,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="D26" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="D26" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E26" s="7" t="s">
+      <c r="F26" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2470,19 +2417,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E27" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2490,19 +2437,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="D28" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="E28" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="F28" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2510,19 +2457,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E29" s="7" t="s">
+      <c r="F29" s="7" t="s">
         <v>124</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2530,19 +2477,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="D30" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E30" s="7" t="s">
+      <c r="F30" s="7" t="s">
         <v>128</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2550,17 +2497,17 @@
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>131</v>
-      </c>
       <c r="D31" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2568,19 +2515,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="D32" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="E32" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="F32" s="7" t="s">
         <v>136</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2588,19 +2535,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="D33" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>140</v>
-      </c>
       <c r="F33" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2608,19 +2555,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="D34" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E34" s="7" t="s">
+      <c r="F34" s="7" t="s">
         <v>143</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2628,19 +2575,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="D35" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E35" s="7" t="s">
+      <c r="F35" s="7" t="s">
         <v>147</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2648,19 +2595,19 @@
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="D36" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E36" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E36" s="7" t="s">
+      <c r="F36" s="7" t="s">
         <v>151</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2668,19 +2615,19 @@
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="D37" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E37" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="D37" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>155</v>
-      </c>
       <c r="F37" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2688,19 +2635,19 @@
         <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C38" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="D38" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E38" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="D38" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E38" s="7" t="s">
+      <c r="F38" s="7" t="s">
         <v>158</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2708,19 +2655,19 @@
         <v>38</v>
       </c>
       <c r="B39" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="D39" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="D39" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E39" s="7" t="s">
+      <c r="F39" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2728,19 +2675,19 @@
         <v>39</v>
       </c>
       <c r="B40" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="D40" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E40" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="D40" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E40" s="7" t="s">
+      <c r="F40" s="7" t="s">
         <v>166</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2748,19 +2695,19 @@
         <v>40</v>
       </c>
       <c r="B41" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="D41" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="D41" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E41" s="7" t="s">
+      <c r="F41" s="7" t="s">
         <v>170</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2768,19 +2715,19 @@
         <v>41</v>
       </c>
       <c r="B42" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="D42" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E42" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="D42" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E42" s="7" t="s">
+      <c r="F42" s="7" t="s">
         <v>174</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2788,19 +2735,19 @@
         <v>42</v>
       </c>
       <c r="B43" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="D43" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E43" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D43" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E43" s="7" t="s">
+      <c r="F43" s="7" t="s">
         <v>178</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2808,19 +2755,19 @@
         <v>43</v>
       </c>
       <c r="B44" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="D44" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E44" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D44" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E44" s="7" t="s">
+      <c r="F44" s="7" t="s">
         <v>182</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2828,19 +2775,19 @@
         <v>44</v>
       </c>
       <c r="B45" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="D45" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E45" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="D45" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E45" s="7" t="s">
+      <c r="F45" s="7" t="s">
         <v>186</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2848,19 +2795,19 @@
         <v>45</v>
       </c>
       <c r="B46" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="D46" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E46" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="D46" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E46" s="7" t="s">
+      <c r="F46" s="7" t="s">
         <v>190</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2868,19 +2815,19 @@
         <v>46</v>
       </c>
       <c r="B47" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C47" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="D47" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E47" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="D47" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E47" s="7" t="s">
+      <c r="F47" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2888,19 +2835,19 @@
         <v>47</v>
       </c>
       <c r="B48" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="D48" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E48" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="D48" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E48" s="7" t="s">
+      <c r="F48" s="7" t="s">
         <v>198</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2908,19 +2855,19 @@
         <v>48</v>
       </c>
       <c r="B49" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="D49" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E49" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="D49" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E49" s="7" t="s">
+      <c r="F49" s="7" t="s">
         <v>202</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2928,19 +2875,19 @@
         <v>49</v>
       </c>
       <c r="B50" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="C50" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="D50" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E50" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="D50" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E50" s="7" t="s">
+      <c r="F50" s="7" t="s">
         <v>206</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2948,19 +2895,19 @@
         <v>50</v>
       </c>
       <c r="B51" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C51" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="D51" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E51" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="D51" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>210</v>
-      </c>
       <c r="F51" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2968,19 +2915,19 @@
         <v>51</v>
       </c>
       <c r="B52" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C52" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="D52" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E52" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="D52" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E52" s="7" t="s">
+      <c r="F52" s="7" t="s">
         <v>213</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2988,19 +2935,19 @@
         <v>52</v>
       </c>
       <c r="B53" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C53" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="D53" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E53" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="D53" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E53" s="7" t="s">
+      <c r="F53" s="7" t="s">
         <v>217</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3008,19 +2955,19 @@
         <v>53</v>
       </c>
       <c r="B54" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C54" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="D54" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E54" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="D54" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E54" s="7" t="s">
+      <c r="F54" s="7" t="s">
         <v>221</v>
-      </c>
-      <c r="F54" s="7" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3028,19 +2975,19 @@
         <v>54</v>
       </c>
       <c r="B55" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C55" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="D55" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E55" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="D55" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E55" s="7" t="s">
+      <c r="F55" s="7" t="s">
         <v>225</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3048,19 +2995,19 @@
         <v>55</v>
       </c>
       <c r="B56" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="D56" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E56" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="D56" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E56" s="7" t="s">
+      <c r="F56" s="7" t="s">
         <v>229</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3068,19 +3015,19 @@
         <v>56</v>
       </c>
       <c r="B57" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="C57" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="D57" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E57" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="D57" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E57" s="7" t="s">
+      <c r="F57" s="7" t="s">
         <v>233</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3088,19 +3035,19 @@
         <v>57</v>
       </c>
       <c r="B58" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C58" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="D58" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E58" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="D58" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E58" s="7" t="s">
+      <c r="F58" s="7" t="s">
         <v>237</v>
-      </c>
-      <c r="F58" s="7" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3109,16 +3056,16 @@
       </c>
       <c r="B59" s="6"/>
       <c r="C59" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E59" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="D59" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E59" s="7" t="s">
+      <c r="F59" s="10" t="s">
         <v>240</v>
-      </c>
-      <c r="F59" s="10" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3126,19 +3073,19 @@
         <v>59</v>
       </c>
       <c r="B60" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="C60" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="C60" s="7" t="s">
-        <v>243</v>
-      </c>
       <c r="D60" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E60" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="E60" s="7" t="s">
+      <c r="F60" s="7" t="s">
         <v>245</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3146,19 +3093,19 @@
         <v>60</v>
       </c>
       <c r="B61" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C61" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="D61" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E61" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="D61" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="E61" s="7" t="s">
+      <c r="F61" s="7" t="s">
         <v>249</v>
-      </c>
-      <c r="F61" s="7" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3166,19 +3113,19 @@
         <v>61</v>
       </c>
       <c r="B62" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="C62" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="D62" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E62" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="D62" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="E62" s="7" t="s">
+      <c r="F62" s="7" t="s">
         <v>253</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3186,19 +3133,19 @@
         <v>62</v>
       </c>
       <c r="B63" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="C63" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="D63" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E63" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="D63" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="E63" s="7" t="s">
+      <c r="F63" s="7" t="s">
         <v>257</v>
-      </c>
-      <c r="F63" s="7" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3206,19 +3153,19 @@
         <v>63</v>
       </c>
       <c r="B64" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C64" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="D64" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E64" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="D64" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="E64" s="7" t="s">
+      <c r="F64" s="7" t="s">
         <v>261</v>
-      </c>
-      <c r="F64" s="7" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3226,19 +3173,19 @@
         <v>64</v>
       </c>
       <c r="B65" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="C65" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="D65" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E65" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="D65" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="E65" s="7" t="s">
+      <c r="F65" s="7" t="s">
         <v>265</v>
-      </c>
-      <c r="F65" s="7" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3246,19 +3193,19 @@
         <v>65</v>
       </c>
       <c r="B66" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="C66" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="D66" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E66" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="D66" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="E66" s="7" t="s">
+      <c r="F66" s="7" t="s">
         <v>269</v>
-      </c>
-      <c r="F66" s="7" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3266,19 +3213,19 @@
         <v>66</v>
       </c>
       <c r="B67" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="C67" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="C67" s="7" t="s">
+      <c r="D67" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E67" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="D67" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="E67" s="7" t="s">
+      <c r="F67" s="7" t="s">
         <v>273</v>
-      </c>
-      <c r="F67" s="7" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3286,19 +3233,19 @@
         <v>67</v>
       </c>
       <c r="B68" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="C68" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="D68" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E68" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="D68" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="E68" s="7" t="s">
+      <c r="F68" s="7" t="s">
         <v>277</v>
-      </c>
-      <c r="F68" s="7" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3306,19 +3253,19 @@
         <v>68</v>
       </c>
       <c r="B69" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C69" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="D69" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E69" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="D69" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="E69" s="7" t="s">
+      <c r="F69" s="7" t="s">
         <v>281</v>
-      </c>
-      <c r="F69" s="7" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3326,19 +3273,19 @@
         <v>69</v>
       </c>
       <c r="B70" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="C70" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="D70" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="D70" s="8" t="s">
+      <c r="E70" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="E70" s="7" t="s">
+      <c r="F70" s="7" t="s">
         <v>286</v>
-      </c>
-      <c r="F70" s="7" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3346,19 +3293,19 @@
         <v>70</v>
       </c>
       <c r="B71" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C71" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="C71" s="7" t="s">
+      <c r="D71" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="E71" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="D71" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="E71" s="7" t="s">
+      <c r="F71" s="7" t="s">
         <v>290</v>
-      </c>
-      <c r="F71" s="7" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3366,19 +3313,19 @@
         <v>71</v>
       </c>
       <c r="B72" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="C72" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="C72" s="7" t="s">
+      <c r="D72" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E72" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="D72" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="E72" s="7" t="s">
+      <c r="F72" s="7" t="s">
         <v>294</v>
-      </c>
-      <c r="F72" s="7" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3386,19 +3333,19 @@
         <v>72</v>
       </c>
       <c r="B73" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="C73" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="C73" s="7" t="s">
+      <c r="D73" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E73" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="D73" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="E73" s="7" t="s">
+      <c r="F73" s="7" t="s">
         <v>298</v>
-      </c>
-      <c r="F73" s="7" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3406,19 +3353,19 @@
         <v>73</v>
       </c>
       <c r="B74" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="C74" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="C74" s="7" t="s">
+      <c r="D74" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E74" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="D74" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="E74" s="7" t="s">
-        <v>302</v>
-      </c>
       <c r="F74" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3426,19 +3373,19 @@
         <v>74</v>
       </c>
       <c r="B75" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="C75" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="C75" s="7" t="s">
+      <c r="D75" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E75" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="D75" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="E75" s="7" t="s">
-        <v>305</v>
-      </c>
       <c r="F75" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3446,19 +3393,19 @@
         <v>75</v>
       </c>
       <c r="B76" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="C76" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="D76" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E76" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="D76" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="E76" s="7" t="s">
-        <v>308</v>
-      </c>
       <c r="F76" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3466,19 +3413,19 @@
         <v>76</v>
       </c>
       <c r="B77" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="C77" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="C77" s="7" t="s">
+      <c r="D77" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E77" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="D77" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="E77" s="7" t="s">
+      <c r="F77" s="7" t="s">
         <v>311</v>
-      </c>
-      <c r="F77" s="7" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3486,19 +3433,19 @@
         <v>77</v>
       </c>
       <c r="B78" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="C78" s="11" t="s">
         <v>313</v>
       </c>
-      <c r="C78" s="11" t="s">
+      <c r="D78" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E78" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="D78" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="E78" s="7" t="s">
+      <c r="F78" s="7" t="s">
         <v>315</v>
-      </c>
-      <c r="F78" s="7" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3506,19 +3453,19 @@
         <v>78</v>
       </c>
       <c r="B79" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="C79" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="C79" s="11" t="s">
+      <c r="D79" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E79" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="D79" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="E79" s="7" t="s">
+      <c r="F79" s="7" t="s">
         <v>319</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3526,19 +3473,19 @@
         <v>79</v>
       </c>
       <c r="B80" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="C80" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="C80" s="11" t="s">
+      <c r="D80" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E80" s="7" t="s">
         <v>322</v>
       </c>
-      <c r="D80" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="E80" s="7" t="s">
+      <c r="F80" s="7" t="s">
         <v>323</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3546,19 +3493,19 @@
         <v>80</v>
       </c>
       <c r="B81" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="C81" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="C81" s="12" t="s">
+      <c r="D81" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E81" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="D81" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="E81" s="7" t="s">
+      <c r="F81" s="7" t="s">
         <v>327</v>
-      </c>
-      <c r="F81" s="7" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3566,19 +3513,19 @@
         <v>81</v>
       </c>
       <c r="B82" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="C82" s="12" t="s">
         <v>329</v>
       </c>
-      <c r="C82" s="12" t="s">
+      <c r="D82" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E82" s="7" t="s">
         <v>330</v>
       </c>
-      <c r="D82" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="E82" s="7" t="s">
+      <c r="F82" s="7" t="s">
         <v>331</v>
-      </c>
-      <c r="F82" s="7" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3586,19 +3533,19 @@
         <v>82</v>
       </c>
       <c r="B83" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="C83" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="C83" s="12" t="s">
+      <c r="D83" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E83" s="7" t="s">
         <v>334</v>
       </c>
-      <c r="D83" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="E83" s="7" t="s">
+      <c r="F83" s="7" t="s">
         <v>335</v>
-      </c>
-      <c r="F83" s="7" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3606,19 +3553,19 @@
         <v>83</v>
       </c>
       <c r="B84" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="C84" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="C84" s="9" t="s">
+      <c r="D84" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E84" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="D84" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="E84" s="7" t="s">
+      <c r="F84" s="7" t="s">
         <v>339</v>
-      </c>
-      <c r="F84" s="7" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3626,19 +3573,19 @@
         <v>84</v>
       </c>
       <c r="B85" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="C85" s="9" t="s">
         <v>341</v>
       </c>
-      <c r="C85" s="9" t="s">
+      <c r="D85" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E85" s="7" t="s">
         <v>342</v>
       </c>
-      <c r="D85" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="E85" s="7" t="s">
+      <c r="F85" s="7" t="s">
         <v>343</v>
-      </c>
-      <c r="F85" s="7" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3646,19 +3593,19 @@
         <v>85</v>
       </c>
       <c r="B86" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="C86" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="C86" s="9" t="s">
+      <c r="D86" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E86" s="7" t="s">
         <v>346</v>
       </c>
-      <c r="D86" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="E86" s="7" t="s">
-        <v>347</v>
-      </c>
       <c r="F86" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3666,19 +3613,19 @@
         <v>86</v>
       </c>
       <c r="B87" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="C87" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="C87" s="9" t="s">
+      <c r="D87" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E87" s="7" t="s">
         <v>349</v>
       </c>
-      <c r="D87" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="E87" s="7" t="s">
+      <c r="F87" s="7" t="s">
         <v>350</v>
-      </c>
-      <c r="F87" s="7" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3686,19 +3633,19 @@
         <v>87</v>
       </c>
       <c r="B88" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="C88" s="9" t="s">
         <v>352</v>
       </c>
-      <c r="C88" s="9" t="s">
+      <c r="D88" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E88" s="7" t="s">
         <v>353</v>
       </c>
-      <c r="D88" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="E88" s="7" t="s">
-        <v>354</v>
-      </c>
       <c r="F88" s="7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3706,19 +3653,19 @@
         <v>88</v>
       </c>
       <c r="B89" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="C89" s="9" t="s">
         <v>355</v>
       </c>
-      <c r="C89" s="9" t="s">
+      <c r="D89" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="E89" s="9" t="s">
         <v>356</v>
       </c>
-      <c r="D89" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="E89" s="9" t="s">
+      <c r="F89" s="9" t="s">
         <v>357</v>
-      </c>
-      <c r="F89" s="9" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3726,19 +3673,19 @@
         <v>89</v>
       </c>
       <c r="B90" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="C90" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="C90" s="9" t="s">
+      <c r="D90" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E90" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="D90" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="E90" s="7" t="s">
+      <c r="F90" s="7" t="s">
         <v>361</v>
-      </c>
-      <c r="F90" s="7" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3746,19 +3693,19 @@
         <v>90</v>
       </c>
       <c r="B91" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="C91" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="C91" s="9" t="s">
+      <c r="D91" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E91" s="7" t="s">
         <v>364</v>
       </c>
-      <c r="D91" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="E91" s="7" t="s">
-        <v>365</v>
-      </c>
       <c r="F91" s="7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3766,19 +3713,19 @@
         <v>91</v>
       </c>
       <c r="B92" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="C92" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="C92" s="9" t="s">
+      <c r="D92" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E92" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="D92" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="E92" s="7" t="s">
+      <c r="F92" s="7" t="s">
         <v>368</v>
-      </c>
-      <c r="F92" s="7" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3786,19 +3733,19 @@
         <v>92</v>
       </c>
       <c r="B93" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="C93" s="9" t="s">
         <v>370</v>
       </c>
-      <c r="C93" s="9" t="s">
+      <c r="D93" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E93" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="D93" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="E93" s="7" t="s">
+      <c r="F93" s="7" t="s">
         <v>372</v>
-      </c>
-      <c r="F93" s="7" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3806,19 +3753,19 @@
         <v>93</v>
       </c>
       <c r="B94" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="C94" s="9" t="s">
         <v>374</v>
       </c>
-      <c r="C94" s="9" t="s">
+      <c r="D94" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E94" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="D94" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="E94" s="7" t="s">
+      <c r="F94" s="7" t="s">
         <v>376</v>
-      </c>
-      <c r="F94" s="7" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3826,19 +3773,19 @@
         <v>94</v>
       </c>
       <c r="B95" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="C95" s="9" t="s">
         <v>378</v>
       </c>
-      <c r="C95" s="9" t="s">
+      <c r="D95" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E95" s="7" t="s">
         <v>379</v>
       </c>
-      <c r="D95" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="E95" s="7" t="s">
+      <c r="F95" s="7" t="s">
         <v>380</v>
-      </c>
-      <c r="F95" s="7" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3846,19 +3793,19 @@
         <v>95</v>
       </c>
       <c r="B96" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="C96" s="9" t="s">
         <v>382</v>
       </c>
-      <c r="C96" s="9" t="s">
+      <c r="D96" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E96" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="D96" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="E96" s="7" t="s">
+      <c r="F96" s="7" t="s">
         <v>384</v>
-      </c>
-      <c r="F96" s="7" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3866,19 +3813,19 @@
         <v>96</v>
       </c>
       <c r="B97" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="C97" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="C97" s="9" t="s">
+      <c r="D97" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E97" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="D97" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="E97" s="7" t="s">
-        <v>388</v>
-      </c>
       <c r="F97" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3886,19 +3833,19 @@
         <v>97</v>
       </c>
       <c r="B98" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="C98" s="9" t="s">
         <v>389</v>
       </c>
-      <c r="C98" s="9" t="s">
+      <c r="D98" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E98" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="D98" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="E98" s="7" t="s">
-        <v>391</v>
-      </c>
       <c r="F98" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3907,16 +3854,16 @@
       </c>
       <c r="B99" s="6"/>
       <c r="C99" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="D99" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="E99" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="D99" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="E99" s="15" t="s">
-        <v>393</v>
-      </c>
       <c r="F99" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3925,16 +3872,16 @@
       </c>
       <c r="B100" s="6"/>
       <c r="C100" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="D100" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="E100" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="D100" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="E100" s="8" t="s">
-        <v>395</v>
-      </c>
       <c r="F100" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3943,16 +3890,16 @@
       </c>
       <c r="B101" s="6"/>
       <c r="C101" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="D101" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="E101" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="D101" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="E101" s="7" t="s">
-        <v>397</v>
-      </c>
       <c r="F101" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3961,16 +3908,16 @@
       </c>
       <c r="B102" s="6"/>
       <c r="C102" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="D102" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="E102" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="D102" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="E102" s="7" t="s">
-        <v>399</v>
-      </c>
       <c r="F102" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3978,19 +3925,19 @@
         <v>102</v>
       </c>
       <c r="B103" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="C103" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="C103" s="16" t="s">
+      <c r="D103" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E103" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="D103" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="E103" s="7" t="s">
+      <c r="F103" s="7" t="s">
         <v>402</v>
-      </c>
-      <c r="F103" s="7" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3998,206 +3945,142 @@
         <v>103</v>
       </c>
       <c r="B104" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="C104" s="17" t="s">
         <v>404</v>
       </c>
-      <c r="C104" s="17" t="s">
+      <c r="D104" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="E104" s="7" t="s">
         <v>405</v>
       </c>
-      <c r="D104" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="E104" s="7" t="s">
+      <c r="F104" s="18" t="s">
         <v>406</v>
       </c>
-      <c r="F104" s="18" t="s">
+    </row>
+    <row r="105" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="19">
+        <v>104</v>
+      </c>
+      <c r="B105" s="6" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="24" t="s">
+      <c r="C105" s="7" t="s">
         <v>408</v>
       </c>
-      <c r="B105" s="25"/>
-      <c r="C105" s="25"/>
-      <c r="D105" s="25"/>
-      <c r="E105" s="25"/>
-      <c r="F105" s="26"/>
+      <c r="D105" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E105" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="F105" s="7" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="106" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D106" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E106" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F106" s="3" t="s">
-        <v>5</v>
+      <c r="A106" s="19">
+        <v>105</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="C106" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="D106" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="E106" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="F106" s="7" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="19">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>75</v>
+        <v>284</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="F107" s="7" t="s">
-        <v>112</v>
+        <v>417</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="19">
-        <v>2</v>
-      </c>
-      <c r="B108" s="6" t="s">
-        <v>412</v>
-      </c>
-      <c r="C108" s="8" t="s">
-        <v>413</v>
-      </c>
-      <c r="D108" s="14" t="s">
-        <v>244</v>
+      <c r="A108" s="5">
+        <v>107</v>
+      </c>
+      <c r="B108" s="20" t="s">
+        <v>418</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="D108" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="19">
-        <v>3</v>
-      </c>
-      <c r="B109" s="6" t="s">
-        <v>416</v>
+      <c r="A109" s="5">
+        <v>108</v>
+      </c>
+      <c r="B109" s="20" t="s">
+        <v>422</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>417</v>
-      </c>
-      <c r="D109" s="8" t="s">
-        <v>285</v>
+        <v>423</v>
+      </c>
+      <c r="D109" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>418</v>
+        <v>424</v>
       </c>
       <c r="F109" s="7" t="s">
-        <v>419</v>
+        <v>425</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="27" t="s">
-        <v>420</v>
-      </c>
-      <c r="B110" s="28"/>
-      <c r="C110" s="28"/>
-      <c r="D110" s="28"/>
-      <c r="E110" s="28"/>
-      <c r="F110" s="29"/>
-    </row>
-    <row r="111" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D111" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F111" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="5">
-        <v>1</v>
-      </c>
-      <c r="B112" s="20" t="s">
-        <v>421</v>
-      </c>
-      <c r="C112" s="7" t="s">
-        <v>422</v>
-      </c>
-      <c r="D112" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E112" s="7" t="s">
-        <v>423</v>
-      </c>
-      <c r="F112" s="7" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="5">
-        <v>2</v>
-      </c>
-      <c r="B113" s="20" t="s">
-        <v>425</v>
-      </c>
-      <c r="C113" s="7" t="s">
+      <c r="A110" s="5">
+        <v>109</v>
+      </c>
+      <c r="B110" s="20" t="s">
         <v>426</v>
       </c>
-      <c r="D113" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E113" s="7" t="s">
+      <c r="C110" s="7" t="s">
         <v>427</v>
       </c>
-      <c r="F113" s="7" t="s">
+      <c r="D110" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E110" s="7" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="5">
-        <v>3</v>
-      </c>
-      <c r="B114" s="20" t="s">
+      <c r="F110" s="7" t="s">
         <v>429</v>
       </c>
-      <c r="C114" s="7" t="s">
-        <v>430</v>
-      </c>
-      <c r="D114" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="E114" s="7" t="s">
-        <v>431</v>
-      </c>
-      <c r="F114" s="7" t="s">
-        <v>432</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A105:F105"/>
-    <mergeCell ref="A110:F110"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>